<commit_message>
Use ExcelDna.Registration and Tasks directly
</commit_message>
<xml_diff>
--- a/SampleExcelBook.xlsx
+++ b/SampleExcelBook.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewBridge\source\repos\HangingExcelDNA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ExcelDna\UserSamples\AndrewBridge\HangingExcelDNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A27C84-6181-470F-B524-20F12FE2659F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236A7BB4-7AE0-4862-A03D-926C6FED5BB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45144" yWindow="2040" windowWidth="22572" windowHeight="17280" activeTab="1" xr2:uid="{6151E36E-2621-45B9-8525-B6D9CCB47B60}"/>
+    <workbookView xWindow="4845" yWindow="1710" windowWidth="18900" windowHeight="11055" xr2:uid="{6151E36E-2621-45B9-8525-B6D9CCB47B60}"/>
   </bookViews>
   <sheets>
     <sheet name="Many calls" sheetId="1" r:id="rId1"/>
     <sheet name="Single call" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -500,16 +499,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE1AE6A-8F34-43B8-9BA6-0CB276E5409B}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>42984</v>
       </c>
@@ -519,7 +518,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -527,7 +526,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +539,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -553,7 +552,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -566,7 +565,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -579,7 +578,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -592,7 +591,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,7 +604,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -618,7 +617,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -631,7 +630,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,7 +643,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -657,7 +656,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -670,7 +669,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -683,7 +682,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -696,7 +695,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -709,7 +708,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -722,7 +721,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -735,7 +734,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -748,7 +747,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -761,7 +760,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -774,7 +773,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -787,7 +786,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -800,7 +799,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -813,7 +812,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -826,7 +825,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -839,7 +838,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -852,7 +851,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -865,7 +864,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -887,13 +886,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37AE96A-AE92-4515-8CC5-FDDE8E5C0E6D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
         <f t="array" ref="A1">_xll.hangexcel_spam("Test", "2018-09-03")</f>
         <v>All complete</v>

</xml_diff>